<commit_message>
testing system now reads in fertiliser applications and passes into simulation and reads observed data and plots on graphs.
</commit_message>
<xml_diff>
--- a/TestComponents/TestSets/WS2/FieldConfigs.xlsx
+++ b/TestComponents/TestSets/WS2/FieldConfigs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHubRepos\SVSModelBuildDeploy\TestComponents\TestSets\WS2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79148153-60A2-459D-9993-A931AD1D3A48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BA61F1D-E6DD-45BE-92D3-226FDD2BB33A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11325" xr2:uid="{D68C7BAB-80DE-42A0-A5F7-D611BF3989D6}"/>
+    <workbookView xWindow="-16320" yWindow="-5925" windowWidth="16440" windowHeight="28440" xr2:uid="{D68C7BAB-80DE-42A0-A5F7-D611BF3989D6}"/>
   </bookViews>
   <sheets>
     <sheet name="Lovett" sheetId="1" r:id="rId1"/>
@@ -39,6 +39,7 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
+    <author>tc={BF07AE18-3302-44B1-90E2-ECD34E6B1A3E}</author>
     <author>tc={E0B776FB-25BE-456C-A03E-84268975A6A3}</author>
     <author>tc={D76D8C4D-C9E1-4F7F-9BCF-3C8848450443}</author>
     <author>tc={EFA979EE-6139-4898-A383-E5761EECE235}</author>
@@ -50,7 +51,15 @@
     <author>tc={41971706-E29E-4BB2-BCA0-94F2423467A9}</author>
   </authors>
   <commentList>
-    <comment ref="C6" authorId="0" shapeId="0" xr:uid="{E0B776FB-25BE-456C-A03E-84268975A6A3}">
+    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{BF07AE18-3302-44B1-90E2-ECD34E6B1A3E}">
+      <text>
+        <t xml:space="preserve">[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    This needs to be our best guess, based on the observations we have, at what the mineral N was on the day the prior crop was harvested.  </t>
+      </text>
+    </comment>
+    <comment ref="C6" authorId="1" shapeId="0" xr:uid="{E0B776FB-25BE-456C-A03E-84268975A6A3}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -58,7 +67,7 @@
     Mean of 0-15 and 15-30 cm @ the start of the season.</t>
       </text>
     </comment>
-    <comment ref="C12" authorId="1" shapeId="0" xr:uid="{D76D8C4D-C9E1-4F7F-9BCF-3C8848450443}">
+    <comment ref="C12" authorId="2" shapeId="0" xr:uid="{D76D8C4D-C9E1-4F7F-9BCF-3C8848450443}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -66,7 +75,7 @@
     1 m depth </t>
       </text>
     </comment>
-    <comment ref="C17" authorId="2" shapeId="0" xr:uid="{EFA979EE-6139-4898-A383-E5761EECE235}">
+    <comment ref="C17" authorId="3" shapeId="0" xr:uid="{EFA979EE-6139-4898-A383-E5761EECE235}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -74,7 +83,7 @@
     Fresh Yield</t>
       </text>
     </comment>
-    <comment ref="D17" authorId="3" shapeId="0" xr:uid="{83393D6E-3494-420C-925F-BE903A610E9A}">
+    <comment ref="D17" authorId="4" shapeId="0" xr:uid="{83393D6E-3494-420C-925F-BE903A610E9A}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -82,7 +91,7 @@
     @ 14% moisture - not specified in the tool</t>
       </text>
     </comment>
-    <comment ref="E17" authorId="4" shapeId="0" xr:uid="{ECF7E98D-4566-4A78-8194-A4B2EBCB33AD}">
+    <comment ref="E17" authorId="5" shapeId="0" xr:uid="{ECF7E98D-4566-4A78-8194-A4B2EBCB33AD}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -90,7 +99,7 @@
     @ 14% moisture</t>
       </text>
     </comment>
-    <comment ref="C20" authorId="5" shapeId="0" xr:uid="{B9626CDC-644A-49BA-B1FD-6B5F8316418E}">
+    <comment ref="C20" authorId="6" shapeId="0" xr:uid="{B9626CDC-644A-49BA-B1FD-6B5F8316418E}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -98,7 +107,7 @@
     Assuming good moisture 0-15 cm</t>
       </text>
     </comment>
-    <comment ref="C28" authorId="6" shapeId="0" xr:uid="{CC4D6E8B-A0AF-4A8D-ADFE-33058901246C}">
+    <comment ref="C28" authorId="7" shapeId="0" xr:uid="{CC4D6E8B-A0AF-4A8D-ADFE-33058901246C}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -106,7 +115,7 @@
     @ 14% moisture - not specified in the tool</t>
       </text>
     </comment>
-    <comment ref="D28" authorId="7" shapeId="0" xr:uid="{4A24CD7E-B336-4CA9-8481-C31D95EDC06A}">
+    <comment ref="D28" authorId="8" shapeId="0" xr:uid="{4A24CD7E-B336-4CA9-8481-C31D95EDC06A}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -114,7 +123,7 @@
     @ 14% moisture</t>
       </text>
     </comment>
-    <comment ref="C39" authorId="8" shapeId="0" xr:uid="{41971706-E29E-4BB2-BCA0-94F2423467A9}">
+    <comment ref="C39" authorId="9" shapeId="0" xr:uid="{41971706-E29E-4BB2-BCA0-94F2423467A9}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -559,7 +568,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -583,6 +592,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="7">
@@ -822,6 +837,7 @@
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Hamish Brown" id="{CC0C7681-170C-4EE9-B4B4-F493C79AE532}" userId="S::Hamish.Brown@plantandfood.co.nz::e7bf7c8e-b50e-4274-a9c9-19d596943665" providerId="AD"/>
   <person displayName="Steven Dellow" id="{2BEBAB2E-91BA-40B3-BEE5-7E6784164FBF}" userId="S::Steven.Dellow@plantandfood.co.nz::d553972a-da9e-49e5-8995-75e3e6c4a535" providerId="AD"/>
 </personList>
 </file>
@@ -1123,6 +1139,9 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="B3" dT="2024-01-10T04:34:55.62" personId="{CC0C7681-170C-4EE9-B4B4-F493C79AE532}" id="{BF07AE18-3302-44B1-90E2-ECD34E6B1A3E}">
+    <text xml:space="preserve">This needs to be our best guess, based on the observations we have, at what the mineral N was on the day the prior crop was harvested.  </text>
+  </threadedComment>
   <threadedComment ref="C6" dT="2023-10-26T00:51:32.63" personId="{2BEBAB2E-91BA-40B3-BEE5-7E6784164FBF}" id="{E0B776FB-25BE-456C-A03E-84268975A6A3}">
     <text>Mean of 0-15 and 15-30 cm @ the start of the season.</text>
   </threadedComment>
@@ -1198,11 +1217,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C27FB4FB-42CF-4046-81E6-EAE466E39234}">
   <dimension ref="A1:Q57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" sqref="A1:XFD48"/>
+      <selection pane="bottomRight" activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1244,16 +1263,16 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="24"/>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="2">
         <v>50</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="2">
         <v>50</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="2">
         <v>50</v>
       </c>
     </row>

</xml_diff>